<commit_message>
Revised version: described search strategy + added Cvasciuc 2020 paper
</commit_message>
<xml_diff>
--- a/Input/StudyOverview.xlsx
+++ b/Input/StudyOverview.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$19</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>ref</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>total_cases</t>
+  </si>
+  <si>
+    <t>Northern Ireland</t>
+  </si>
+  <si>
+    <t>Cvasciuc 2020</t>
   </si>
 </sst>
 </file>
@@ -450,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,113 +759,142 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="C11">
         <v>2020</v>
       </c>
       <c r="D11">
-        <v>1995</v>
+        <v>2010</v>
       </c>
       <c r="E11">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="F11" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="G11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H11">
-        <v>355</v>
+        <v>64</v>
       </c>
       <c r="I11">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
       </c>
       <c r="C12">
         <v>2020</v>
       </c>
       <c r="D12">
+        <v>1995</v>
+      </c>
+      <c r="E12">
+        <v>2017</v>
+      </c>
+      <c r="F12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>355</v>
+      </c>
+      <c r="I12">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>2020</v>
+      </c>
+      <c r="D13">
         <v>2003</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>2014</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F13" t="s">
         <v>6</v>
-      </c>
-      <c r="G12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12">
-        <v>72</v>
-      </c>
-      <c r="I12">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13">
-        <v>2021</v>
-      </c>
-      <c r="D13">
-        <v>1977</v>
-      </c>
-      <c r="E13">
-        <v>2015</v>
-      </c>
-      <c r="F13" t="s">
-        <v>3</v>
       </c>
       <c r="G13" t="s">
         <v>9</v>
       </c>
       <c r="H13">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="I13">
-        <v>567</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14">
         <v>2021</v>
       </c>
       <c r="D14">
-        <v>2012</v>
+        <v>1977</v>
       </c>
       <c r="E14">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="F14" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G14" t="s">
         <v>9</v>
       </c>
       <c r="H14">
+        <v>64</v>
+      </c>
+      <c r="I14">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>2021</v>
+      </c>
+      <c r="D15">
+        <v>2012</v>
+      </c>
+      <c r="E15">
+        <v>2019</v>
+      </c>
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15">
         <v>773</v>
       </c>
-      <c r="I14">
+      <c r="I15">
         <v>239</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J18">
+  <autoFilter ref="A1:J19">
     <sortState ref="A2:N14">
       <sortCondition ref="C1:C18"/>
     </sortState>

</xml_diff>